<commit_message>
Update Data Mudik Indonesia 2022.xlsx
</commit_message>
<xml_diff>
--- a/Indonesia Mudik 2022/Data Mudik Indonesia 2022.xlsx
+++ b/Indonesia Mudik 2022/Data Mudik Indonesia 2022.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dataviz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Tableau\Indonesia Mudik 2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB33957-452A-4E9E-ADB9-52C2760D3442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9335D102-E95C-4273-91E4-2AD6F033F4DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="7" xr2:uid="{CAA1E064-0EF9-4C3F-BC3E-306150A99F8C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="68">
   <si>
     <t>Pertamina Dex</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Juta Orang (Pengguna Kendaraan)</t>
+  </si>
+  <si>
+    <t>Yogyakarta</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1234,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:O5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,7 +1404,7 @@
         <v>4540720</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="I4" s="7">
         <v>14.7</v>
@@ -1465,7 +1468,7 @@
         <v>1977425</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>18</v>
+        <v>67</v>
       </c>
       <c r="I6" s="7">
         <v>3.9</v>

</xml_diff>